<commit_message>
ng: add ogun forms
</commit_message>
<xml_diff>
--- a/ONCHO/Impact Assessments/Nigeria/2024/ogun/ng_oncho_stop_202403_1_site_ogun.xlsx
+++ b/ONCHO/Impact Assessments/Nigeria/2024/ogun/ng_oncho_stop_202403_1_site_ogun.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\ONCHO\Impact Assessments\Nigeria\2024\ekiti\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\ONCHO\Impact Assessments\Nigeria\2024\ogun\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2296674B-B07B-4D45-BB0D-C7676C5226EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{349068A4-EC6A-4ED8-8A2A-9C4F369C3717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="154">
   <si>
     <t>type</t>
   </si>
@@ -383,121 +383,118 @@
     <t>English</t>
   </si>
   <si>
-    <t>IROKO</t>
-  </si>
-  <si>
-    <t>EKITI</t>
-  </si>
-  <si>
-    <t>ADO-EKITI</t>
-  </si>
-  <si>
-    <t>EKITI EAST</t>
-  </si>
-  <si>
-    <t>EKITI SOUTH-WEST</t>
-  </si>
-  <si>
-    <t>EKITI WEST</t>
-  </si>
-  <si>
-    <t>GBONYIN</t>
-  </si>
-  <si>
-    <t>IDO-OSI</t>
-  </si>
-  <si>
-    <t>IJERO</t>
-  </si>
-  <si>
-    <t>IKERE</t>
-  </si>
-  <si>
-    <t>IKOLE</t>
-  </si>
-  <si>
-    <t>IREPODUN/IFELODUN</t>
-  </si>
-  <si>
-    <t>ISE/ORUN</t>
-  </si>
-  <si>
-    <t>MOBA</t>
-  </si>
-  <si>
-    <t>OWO</t>
-  </si>
-  <si>
-    <t>OYE</t>
-  </si>
-  <si>
-    <t>IGBODOGI</t>
-  </si>
-  <si>
-    <t>IRORO</t>
-  </si>
-  <si>
-    <t>OMUO-EKITI</t>
-  </si>
-  <si>
-    <t>IGBARA ODO</t>
-  </si>
-  <si>
-    <t>ERIO EKITI</t>
-  </si>
-  <si>
-    <t>OKE MESI</t>
-  </si>
-  <si>
-    <t>AISEGBA</t>
-  </si>
-  <si>
-    <t>ODE-EKITI</t>
-  </si>
-  <si>
-    <t>ORIN</t>
-  </si>
-  <si>
-    <t>ARAROMI</t>
-  </si>
-  <si>
-    <t>OKO OISA</t>
-  </si>
-  <si>
-    <t>IJESA-ISU</t>
-  </si>
-  <si>
-    <t>IYEMERO</t>
-  </si>
-  <si>
-    <t>IWOROKO</t>
-  </si>
-  <si>
-    <t>ASOLO</t>
-  </si>
-  <si>
-    <t>ISE</t>
-  </si>
-  <si>
-    <t>EPE</t>
-  </si>
-  <si>
-    <t>IGBE</t>
-  </si>
-  <si>
-    <t>AIYEDE</t>
-  </si>
-  <si>
-    <t>IJEMOSO</t>
-  </si>
-  <si>
-    <t>ILEMESO EKITI</t>
-  </si>
-  <si>
-    <t>ng_oncho_stop_202403_1_site</t>
-  </si>
-  <si>
-    <t>(2024 Mar) - 1. Site Form</t>
+    <t>ng_oncho_stop_202403_1_site_ogun</t>
+  </si>
+  <si>
+    <t>(2024 Mar) - 1. Site Form - Ogun State</t>
+  </si>
+  <si>
+    <t>OGUN</t>
+  </si>
+  <si>
+    <t>ABEOKUTA NORTH</t>
+  </si>
+  <si>
+    <t>ADO ODO/OTA</t>
+  </si>
+  <si>
+    <t>ADO-ODO/OTA (BADAGRY)</t>
+  </si>
+  <si>
+    <t>EGBADO NORTH</t>
+  </si>
+  <si>
+    <t>IFO</t>
+  </si>
+  <si>
+    <t>IJEBU EAST</t>
+  </si>
+  <si>
+    <t>IJEBU NORTH</t>
+  </si>
+  <si>
+    <t>IJEBU-ODE</t>
+  </si>
+  <si>
+    <t>IMEKO AFON</t>
+  </si>
+  <si>
+    <t>OBAFEMI O</t>
+  </si>
+  <si>
+    <t>OBAFEMI OWODE</t>
+  </si>
+  <si>
+    <t>ODEDA</t>
+  </si>
+  <si>
+    <t>ODOGBOLU</t>
+  </si>
+  <si>
+    <t>SAGAMU</t>
+  </si>
+  <si>
+    <t>YEWA SOUTH</t>
+  </si>
+  <si>
+    <t>ATAPA IKOYI</t>
+  </si>
+  <si>
+    <t>IDIMU</t>
+  </si>
+  <si>
+    <t>SEJE</t>
+  </si>
+  <si>
+    <t>EGGUA</t>
+  </si>
+  <si>
+    <t>SAALA-ORILE</t>
+  </si>
+  <si>
+    <t>ASANI</t>
+  </si>
+  <si>
+    <t>OKE-MAKUN</t>
+  </si>
+  <si>
+    <t>AJEGUNLE AWA</t>
+  </si>
+  <si>
+    <t>DAMOLA</t>
+  </si>
+  <si>
+    <t>MOSINMI</t>
+  </si>
+  <si>
+    <t>IRAWO</t>
+  </si>
+  <si>
+    <t>ALLA SOKA</t>
+  </si>
+  <si>
+    <t>IDOFA</t>
+  </si>
+  <si>
+    <t>AROGUN</t>
+  </si>
+  <si>
+    <t>OLOJO</t>
+  </si>
+  <si>
+    <t>ABULE SET</t>
+  </si>
+  <si>
+    <t>JAGUNA</t>
+  </si>
+  <si>
+    <t>OKUN-OWO</t>
+  </si>
+  <si>
+    <t>ODELEMO</t>
+  </si>
+  <si>
+    <t>IDOGO</t>
   </si>
 </sst>
 </file>
@@ -947,7 +944,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -1415,11 +1412,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F84"/>
+  <dimension ref="A1:F81"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A85" sqref="A85:XFD91"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A23" sqref="A23:XFD81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1712,10 +1709,10 @@
         <v>87</v>
       </c>
       <c r="B23" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C23" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1723,13 +1720,13 @@
         <v>88</v>
       </c>
       <c r="B25" t="s">
+        <v>119</v>
+      </c>
+      <c r="C25" t="s">
+        <v>119</v>
+      </c>
+      <c r="D25" s="9" t="s">
         <v>118</v>
-      </c>
-      <c r="C25" t="s">
-        <v>118</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1737,13 +1734,13 @@
         <v>88</v>
       </c>
       <c r="B26" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C26" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1751,13 +1748,13 @@
         <v>88</v>
       </c>
       <c r="B27" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C27" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1765,13 +1762,13 @@
         <v>88</v>
       </c>
       <c r="B28" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C28" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1779,13 +1776,13 @@
         <v>88</v>
       </c>
       <c r="B29" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C29" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -1793,13 +1790,13 @@
         <v>88</v>
       </c>
       <c r="B30" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C30" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1807,13 +1804,13 @@
         <v>88</v>
       </c>
       <c r="B31" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C31" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1821,13 +1818,13 @@
         <v>88</v>
       </c>
       <c r="B32" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C32" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -1835,13 +1832,13 @@
         <v>88</v>
       </c>
       <c r="B33" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C33" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1849,13 +1846,13 @@
         <v>88</v>
       </c>
       <c r="B34" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C34" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -1863,13 +1860,13 @@
         <v>88</v>
       </c>
       <c r="B35" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C35" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D35" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1877,13 +1874,13 @@
         <v>88</v>
       </c>
       <c r="B36" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C36" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D36" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1891,13 +1888,13 @@
         <v>88</v>
       </c>
       <c r="B37" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C37" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D37" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1905,26 +1902,26 @@
         <v>88</v>
       </c>
       <c r="B38" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C38" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D38" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40" t="s">
-        <v>89</v>
-      </c>
-      <c r="B40" t="s">
-        <v>132</v>
-      </c>
-      <c r="C40" t="s">
-        <v>132</v>
-      </c>
-      <c r="E40" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" t="s">
+        <v>88</v>
+      </c>
+      <c r="B39" t="s">
+        <v>133</v>
+      </c>
+      <c r="C39" t="s">
+        <v>133</v>
+      </c>
+      <c r="D39" t="s">
         <v>118</v>
       </c>
     </row>
@@ -1933,10 +1930,10 @@
         <v>89</v>
       </c>
       <c r="B41" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C41" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E41" t="s">
         <v>119</v>
@@ -1947,13 +1944,13 @@
         <v>89</v>
       </c>
       <c r="B42" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C42" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E42" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1961,13 +1958,13 @@
         <v>89</v>
       </c>
       <c r="B43" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C43" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E43" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1975,13 +1972,13 @@
         <v>89</v>
       </c>
       <c r="B44" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C44" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E44" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1989,13 +1986,13 @@
         <v>89</v>
       </c>
       <c r="B45" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C45" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E45" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -2003,13 +2000,13 @@
         <v>89</v>
       </c>
       <c r="B46" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C46" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E46" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -2017,13 +2014,13 @@
         <v>89</v>
       </c>
       <c r="B47" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C47" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E47" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -2031,13 +2028,13 @@
         <v>89</v>
       </c>
       <c r="B48" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C48" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E48" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -2045,13 +2042,13 @@
         <v>89</v>
       </c>
       <c r="B49" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C49" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E49" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -2059,13 +2056,13 @@
         <v>89</v>
       </c>
       <c r="B50" t="s">
-        <v>116</v>
+        <v>143</v>
       </c>
       <c r="C50" t="s">
-        <v>116</v>
+        <v>143</v>
       </c>
       <c r="E50" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -2073,13 +2070,13 @@
         <v>89</v>
       </c>
       <c r="B51" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C51" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="E51" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -2087,13 +2084,13 @@
         <v>89</v>
       </c>
       <c r="B52" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C52" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="E52" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -2101,13 +2098,13 @@
         <v>89</v>
       </c>
       <c r="B53" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C53" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E53" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -2115,13 +2112,13 @@
         <v>89</v>
       </c>
       <c r="B54" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C54" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E54" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -2129,13 +2126,13 @@
         <v>89</v>
       </c>
       <c r="B55" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C55" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E55" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -2143,13 +2140,13 @@
         <v>89</v>
       </c>
       <c r="B56" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C56" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="E56" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -2157,13 +2154,13 @@
         <v>89</v>
       </c>
       <c r="B57" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C57" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="E57" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -2171,13 +2168,13 @@
         <v>89</v>
       </c>
       <c r="B58" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C58" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="E58" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -2185,13 +2182,13 @@
         <v>89</v>
       </c>
       <c r="B59" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C59" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="E59" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -2199,27 +2196,27 @@
         <v>89</v>
       </c>
       <c r="B60" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C60" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E60" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6">
-      <c r="A61" t="s">
-        <v>89</v>
-      </c>
-      <c r="B61" t="s">
-        <v>152</v>
-      </c>
-      <c r="C61" t="s">
-        <v>152</v>
-      </c>
-      <c r="E61" t="s">
-        <v>131</v>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B62">
+        <v>201</v>
+      </c>
+      <c r="C62">
+        <v>201</v>
+      </c>
+      <c r="F62" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -2227,13 +2224,13 @@
         <v>111</v>
       </c>
       <c r="B63">
-        <v>101</v>
+        <v>202</v>
       </c>
       <c r="C63">
-        <v>101</v>
+        <v>202</v>
       </c>
       <c r="F63" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -2241,13 +2238,13 @@
         <v>111</v>
       </c>
       <c r="B64">
-        <v>102</v>
+        <v>203</v>
       </c>
       <c r="C64">
-        <v>102</v>
+        <v>203</v>
       </c>
       <c r="F64" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -2255,13 +2252,13 @@
         <v>111</v>
       </c>
       <c r="B65">
-        <v>103</v>
+        <v>204</v>
       </c>
       <c r="C65">
-        <v>103</v>
+        <v>204</v>
       </c>
       <c r="F65" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -2269,13 +2266,13 @@
         <v>111</v>
       </c>
       <c r="B66">
-        <v>104</v>
+        <v>205</v>
       </c>
       <c r="C66">
-        <v>104</v>
+        <v>205</v>
       </c>
       <c r="F66" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -2283,13 +2280,13 @@
         <v>111</v>
       </c>
       <c r="B67">
-        <v>105</v>
+        <v>206</v>
       </c>
       <c r="C67">
-        <v>105</v>
+        <v>206</v>
       </c>
       <c r="F67" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -2297,13 +2294,13 @@
         <v>111</v>
       </c>
       <c r="B68">
-        <v>106</v>
+        <v>207</v>
       </c>
       <c r="C68">
-        <v>106</v>
+        <v>207</v>
       </c>
       <c r="F68" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -2311,13 +2308,13 @@
         <v>111</v>
       </c>
       <c r="B69">
-        <v>107</v>
+        <v>208</v>
       </c>
       <c r="C69">
-        <v>107</v>
+        <v>208</v>
       </c>
       <c r="F69" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -2325,13 +2322,13 @@
         <v>111</v>
       </c>
       <c r="B70">
-        <v>108</v>
+        <v>209</v>
       </c>
       <c r="C70">
-        <v>108</v>
+        <v>209</v>
       </c>
       <c r="F70" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -2339,13 +2336,13 @@
         <v>111</v>
       </c>
       <c r="B71">
-        <v>109</v>
+        <v>210</v>
       </c>
       <c r="C71">
-        <v>109</v>
+        <v>210</v>
       </c>
       <c r="F71" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -2353,13 +2350,13 @@
         <v>111</v>
       </c>
       <c r="B72">
-        <v>110</v>
+        <v>211</v>
       </c>
       <c r="C72">
-        <v>110</v>
+        <v>211</v>
       </c>
       <c r="F72" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -2367,13 +2364,13 @@
         <v>111</v>
       </c>
       <c r="B73">
-        <v>111</v>
+        <v>212</v>
       </c>
       <c r="C73">
-        <v>111</v>
+        <v>212</v>
       </c>
       <c r="F73" t="s">
-        <v>116</v>
+        <v>145</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -2381,13 +2378,13 @@
         <v>111</v>
       </c>
       <c r="B74">
-        <v>112</v>
+        <v>213</v>
       </c>
       <c r="C74">
-        <v>112</v>
+        <v>213</v>
       </c>
       <c r="F74" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -2395,13 +2392,13 @@
         <v>111</v>
       </c>
       <c r="B75">
-        <v>113</v>
+        <v>214</v>
       </c>
       <c r="C75">
-        <v>113</v>
+        <v>214</v>
       </c>
       <c r="F75" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -2409,13 +2406,13 @@
         <v>111</v>
       </c>
       <c r="B76">
-        <v>114</v>
+        <v>215</v>
       </c>
       <c r="C76">
-        <v>114</v>
+        <v>215</v>
       </c>
       <c r="F76" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -2423,13 +2420,13 @@
         <v>111</v>
       </c>
       <c r="B77">
-        <v>115</v>
+        <v>216</v>
       </c>
       <c r="C77">
-        <v>115</v>
+        <v>216</v>
       </c>
       <c r="F77" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -2437,13 +2434,13 @@
         <v>111</v>
       </c>
       <c r="B78">
-        <v>116</v>
+        <v>217</v>
       </c>
       <c r="C78">
-        <v>116</v>
+        <v>217</v>
       </c>
       <c r="F78" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -2451,13 +2448,13 @@
         <v>111</v>
       </c>
       <c r="B79">
-        <v>117</v>
+        <v>218</v>
       </c>
       <c r="C79">
-        <v>117</v>
+        <v>218</v>
       </c>
       <c r="F79" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -2465,13 +2462,13 @@
         <v>111</v>
       </c>
       <c r="B80">
-        <v>118</v>
+        <v>219</v>
       </c>
       <c r="C80">
-        <v>118</v>
+        <v>219</v>
       </c>
       <c r="F80" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -2479,61 +2476,19 @@
         <v>111</v>
       </c>
       <c r="B81">
-        <v>119</v>
+        <v>220</v>
       </c>
       <c r="C81">
-        <v>119</v>
+        <v>220</v>
       </c>
       <c r="F81" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6">
-      <c r="A82" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="B82">
-        <v>120</v>
-      </c>
-      <c r="C82">
-        <v>120</v>
-      </c>
-      <c r="F82" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6">
-      <c r="A83" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="B83">
-        <v>121</v>
-      </c>
-      <c r="C83">
-        <v>121</v>
-      </c>
-      <c r="F83" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6">
-      <c r="A84" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="B84">
-        <v>122</v>
-      </c>
-      <c r="C84">
-        <v>122</v>
-      </c>
-      <c r="F84" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A44:E51">
-    <sortCondition ref="A44:A51"/>
-    <sortCondition ref="E44:E51"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A45:E52">
+    <sortCondition ref="A45:A52"/>
+    <sortCondition ref="E45:E52"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2544,7 +2499,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2567,10 +2522,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="13" t="s">
-        <v>154</v>
+        <v>117</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>153</v>
+        <v>116</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>115</v>

</xml_diff>